<commit_message>
Documented and cleaned up code.
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brech\Programs\Python\SMILE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brech\UofA\SPRING2024\DASC400V\SMILE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81149AC7-810E-4FBF-A3DC-3A8D1D959309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDFD4AC-4CBD-4FF7-8764-F6148C7C047B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="performance" sheetId="1" r:id="rId1"/>
     <sheet name="performance (better error)" sheetId="2" r:id="rId2"/>
     <sheet name="performance (updating model)" sheetId="6" r:id="rId3"/>
-    <sheet name="performance (updating model 2)" sheetId="4" r:id="rId4"/>
-    <sheet name="comparison" sheetId="7" r:id="rId5"/>
+    <sheet name="performance (updating model 2)" sheetId="8" r:id="rId4"/>
+    <sheet name="performance (single iteration)" sheetId="4" r:id="rId5"/>
+    <sheet name="comparison" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">performance!$B$1</definedName>
@@ -28,13 +29,28 @@
     <definedName name="_xlchart.v1.5" hidden="1">'performance (updating model)'!$B$2:$B$42</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">'performance (updating model 2)'!$B$1</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">'performance (updating model 2)'!$B$2:$B$42</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'performance (single iteration)'!$B$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'performance (single iteration)'!$B$2:$B$42</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="50">
   <si>
     <t>function</t>
   </si>
@@ -164,15 +180,33 @@
   <si>
     <t>zettl</t>
   </si>
+  <si>
+    <t>Non Sequential</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>More Iterations</t>
+  </si>
+  <si>
+    <t>No Simulation</t>
+  </si>
+  <si>
+    <t>With Simulation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
-  </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,14 +349,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -504,12 +532,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -625,13 +659,9 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </left>
+      <left/>
       <right/>
-      <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color theme="9" tint="0.39997558519241921"/>
       </bottom>
@@ -639,14 +669,25 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
+      <right/>
+      <top style="double">
+        <color theme="9"/>
       </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
+      <bottom style="double">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color theme="9"/>
+      </top>
+      <bottom style="double">
+        <color theme="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -696,16 +737,34 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -752,96 +811,46 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="39">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -905,16 +914,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -930,96 +929,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1165,16 +1074,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1214,114 +1113,13 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1612,6 +1410,75 @@
 </cx:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx5.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.9</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>performance (percentile of final solution)</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>performance (percentile of final solution)</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{FCAF648C-BCD8-4FC6-8F8F-AD9449651503}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:v>performance</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r" underflow="95">
+              <cx:binSize val="1"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling max="25" min="0"/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1772,6 +1639,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
   <cs:axisTitle>
@@ -3297,6 +3204,514 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4508,6 +4923,89 @@
             <xdr:cNvPr id="2" name="Chart 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69C1A084-D703-4567-863B-66B3E53BF989}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2820838" y="181155"/>
+              <a:ext cx="4347713" cy="1449237"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B69D133-3013-4853-9ACA-A93F0C3F93B8}"/>
                 </a:ext>
               </a:extLst>
@@ -4612,6 +5110,20 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{278C5D2F-C027-4FF1-A046-DC4552330D28}" name="Table154" displayName="Table154" ref="A1:B42" totalsRowShown="0">
+  <autoFilter ref="A1:B42" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B42">
+    <sortCondition ref="A1:A42"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{E002C3B7-C504-4333-A1EF-035E0E0AFFED}" name="function"/>
+    <tableColumn id="2" xr3:uid="{A65E59A3-4CF6-4448-BB0E-453F1E6236CD}" name="performance"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{52080A27-5E47-497B-AE7B-01B083BD6675}" name="Table15" displayName="Table15" ref="A1:B42" totalsRowShown="0">
   <autoFilter ref="A1:B42" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B42">
@@ -4620,6 +5132,31 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C9511FA8-C7BD-4EB9-8F73-C4111A1D9E08}" name="function"/>
     <tableColumn id="2" xr3:uid="{AA558980-BE78-4753-95FB-2ECA5918A5C9}" name="performance"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D4C375AD-A49F-4A25-BDB0-BA8D85AB0708}" name="Table136" displayName="Table136" ref="A1:E24" totalsRowCount="1" headerRowDxfId="38" dataDxfId="37" totalsRowDxfId="36">
+  <autoFilter ref="A1:E23" xr:uid="{D4C375AD-A49F-4A25-BDB0-BA8D85AB0708}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B23">
+    <sortCondition ref="A1:A23"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{20C12F79-EC9C-4B67-B29B-E218207662A2}" name="Function" totalsRowLabel="Average" dataDxfId="9" totalsRowDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{3FDD2460-BDB0-41AD-9780-847A01BD0C85}" name="No Simulation" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="3">
+      <totalsRowFormula>AVERAGE(B2:B23)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{C3B36032-78D5-4BD4-A3BC-90942DCC7BB3}" name="With Simulation" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="0">
+      <totalsRowFormula>AVERAGE(C2:C23)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{7B0E1A07-80A4-4403-AC6D-A0CA9635E159}" name="More Iterations" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="2">
+      <totalsRowFormula>AVERAGE(D2:D23)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{55067F11-02F7-4B5A-BE54-54AA0ED0FBDD}" name="Non Sequential" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="1">
+      <totalsRowFormula>AVERAGE(E2:E23)</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4927,8 +5464,8 @@
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B42"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -5275,18 +5812,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B42">
-    <cfRule type="cellIs" dxfId="56" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="between">
       <formula>90</formula>
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="between">
       <formula>90</formula>
       <formula>95</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="greaterThan">
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="lessThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5306,8 +5843,8 @@
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B42"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -5654,14 +6191,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B42">
-    <cfRule type="cellIs" dxfId="52" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="between">
       <formula>80</formula>
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="greaterThan">
       <formula>90</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="lessThan">
       <formula>80</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5681,8 +6218,8 @@
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B42"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -6029,18 +6566,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B42">
-    <cfRule type="cellIs" dxfId="49" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="1" operator="between">
       <formula>90</formula>
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="between">
       <formula>90</formula>
       <formula>95</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="greaterThan">
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="lessThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6054,14 +6591,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1715C3F6-D1B7-48DF-A405-52EAE9C4D8B1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29853F0B-FC67-4154-AECB-D7B48AF83BF1}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B42" sqref="B2:B42"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -6408,18 +6945,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B42">
-    <cfRule type="cellIs" dxfId="45" priority="1" operator="between">
-      <formula>90</formula>
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="between">
+      <formula>95</formula>
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="2" operator="between">
-      <formula>90</formula>
-      <formula>95</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="greaterThan">
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="lessThan">
       <formula>95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6433,880 +6966,1029 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D42686-4F9D-47D4-85A1-99C5AB14B438}">
-  <dimension ref="A1:G41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1715C3F6-D1B7-48DF-A405-52EAE9C4D8B1}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="5.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B2">
+        <v>97.864999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>99.31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>97.81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>99.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>99.13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>99.48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>97.805000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>98.37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>23.754999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>98.594999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>86.77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>96.584999999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>87.504999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>50.034999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>99.504999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>99.974999999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>99.504999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>99.92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>99.784999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>99.83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>99.55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>99.03</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>99.08</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>99.17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>99.19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>98.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>99.72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>43.344999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>46.484999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>55.225000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>48.034999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>89.515000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>98.42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>99.465000000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>98.504999999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>96.844999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>61.005000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <v>99.63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <v>95.86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <v>99.69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42">
+        <v>99.83</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B42">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="between">
+      <formula>95</formula>
+      <formula>99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="greaterThan">
+      <formula>99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="lessThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.3" right="0.3" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="89" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D42686-4F9D-47D4-85A1-99C5AB14B438}">
+  <dimension ref="A1:E67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="21.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3">
+        <v>95.185000000000002</v>
+      </c>
+      <c r="C2" s="3">
+        <v>99.864999999999995</v>
+      </c>
+      <c r="D2" s="3">
+        <v>98.825000000000003</v>
+      </c>
+      <c r="E2" s="3">
+        <v>98.385000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>96.02</v>
+      </c>
+      <c r="C3" s="3">
+        <v>99.2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>98.94</v>
+      </c>
+      <c r="E3" s="3">
+        <v>96.16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>99.94</v>
+      </c>
+      <c r="C4" s="3">
+        <v>93.31</v>
+      </c>
+      <c r="D4" s="3">
+        <v>97.95</v>
+      </c>
+      <c r="E4" s="3">
+        <v>94.37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3">
+        <v>67.38</v>
+      </c>
+      <c r="C5" s="3">
+        <v>98.16</v>
+      </c>
+      <c r="D5" s="3">
+        <v>99.76</v>
+      </c>
+      <c r="E5" s="3">
+        <v>95.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3">
+        <v>94.19</v>
+      </c>
+      <c r="C6" s="3">
+        <v>98.65</v>
+      </c>
+      <c r="D6" s="3">
+        <v>99.18</v>
+      </c>
+      <c r="E6" s="3">
+        <v>98.54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>99.474999999999994</v>
+      </c>
+      <c r="C7" s="3">
+        <v>99.665000000000006</v>
+      </c>
+      <c r="D7" s="3">
+        <v>96.575000000000003</v>
+      </c>
+      <c r="E7" s="3">
+        <v>98.734999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3">
+        <v>98.305000000000007</v>
+      </c>
+      <c r="C8" s="3">
+        <v>98.305000000000007</v>
+      </c>
+      <c r="D8" s="3">
+        <v>93.724999999999994</v>
+      </c>
+      <c r="E8" s="3">
+        <v>99.364999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3">
+        <v>87.52</v>
+      </c>
+      <c r="C9" s="3">
+        <v>99.09</v>
+      </c>
+      <c r="D9" s="3">
+        <v>99.65</v>
+      </c>
+      <c r="E9" s="3">
+        <v>98.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3">
+        <v>65.215000000000003</v>
+      </c>
+      <c r="C10" s="3">
+        <v>99.814999999999998</v>
+      </c>
+      <c r="D10" s="3">
+        <v>96.635000000000005</v>
+      </c>
+      <c r="E10" s="3">
+        <v>99.355000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3">
+        <v>88.12</v>
+      </c>
+      <c r="C11" s="3">
+        <v>96.9</v>
+      </c>
+      <c r="D11" s="3">
+        <v>95.15</v>
+      </c>
+      <c r="E11" s="3">
+        <v>99.08</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="3">
+        <v>98.42</v>
+      </c>
+      <c r="C12" s="3">
+        <v>97.6</v>
+      </c>
+      <c r="D12" s="3">
+        <v>94.42</v>
+      </c>
+      <c r="E12" s="3">
+        <v>96.28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3">
+        <v>86.49</v>
+      </c>
+      <c r="C13" s="3">
+        <v>99.34</v>
+      </c>
+      <c r="D13" s="3">
+        <v>99.2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>99.77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3">
+        <v>76.510000000000005</v>
+      </c>
+      <c r="C14" s="3">
+        <v>99.82</v>
+      </c>
+      <c r="D14" s="3">
+        <v>99.45</v>
+      </c>
+      <c r="E14" s="3">
+        <v>99.52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3">
+        <v>97.405000000000001</v>
+      </c>
+      <c r="C15" s="3">
+        <v>99.245000000000005</v>
+      </c>
+      <c r="D15" s="3">
+        <v>94.72</v>
+      </c>
+      <c r="E15" s="3">
+        <v>98.364999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="3">
+        <v>86.85</v>
+      </c>
+      <c r="C16" s="3">
+        <v>99.73</v>
+      </c>
+      <c r="D16" s="3">
+        <v>98.36</v>
+      </c>
+      <c r="E16" s="3">
+        <v>99.45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="3">
+        <v>93.394999999999996</v>
+      </c>
+      <c r="C17" s="3">
+        <v>98.034999999999997</v>
+      </c>
+      <c r="D17" s="3">
+        <v>89.215000000000003</v>
+      </c>
+      <c r="E17" s="3">
+        <v>98.034999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="3">
+        <v>99.3</v>
+      </c>
+      <c r="C18" s="3">
+        <v>98.26</v>
+      </c>
+      <c r="D18" s="3">
+        <v>98.25</v>
+      </c>
+      <c r="E18" s="3">
+        <v>99.48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="3">
+        <v>91.564999999999998</v>
+      </c>
+      <c r="C19" s="3">
+        <v>99.784999999999997</v>
+      </c>
+      <c r="D19" s="3">
+        <v>98.784999999999997</v>
+      </c>
+      <c r="E19" s="3">
+        <v>99.305000000000007</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="3">
+        <v>99.965000000000003</v>
+      </c>
+      <c r="C20" s="3">
         <v>99.424999999999997</v>
       </c>
-      <c r="C1" s="5">
-        <v>95.185000000000002</v>
-      </c>
-      <c r="D1" s="5">
-        <v>99.385000000000005</v>
-      </c>
-      <c r="E1" s="5">
-        <v>98.605000000000004</v>
-      </c>
-      <c r="F1" s="6">
-        <v>99.385000000000005</v>
-      </c>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="5">
-        <v>99.51</v>
-      </c>
-      <c r="C2" s="5">
-        <v>96.02</v>
-      </c>
-      <c r="D2" s="5">
-        <v>96.56</v>
-      </c>
-      <c r="E2" s="5">
-        <v>99.53</v>
-      </c>
-      <c r="F2" s="6">
-        <v>96.56</v>
-      </c>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5">
-        <v>99.79</v>
-      </c>
-      <c r="C3" s="5">
-        <v>99.94</v>
-      </c>
-      <c r="D3" s="5">
-        <v>98.58</v>
-      </c>
-      <c r="E3" s="5">
-        <v>99.32</v>
-      </c>
-      <c r="F3" s="6">
-        <v>98.58</v>
-      </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="5">
-        <v>99.87</v>
-      </c>
-      <c r="C4" s="5">
-        <v>67.38</v>
-      </c>
-      <c r="D4" s="5">
-        <v>98.31</v>
-      </c>
-      <c r="E4" s="5">
-        <v>99.02</v>
-      </c>
-      <c r="F4" s="6">
-        <v>98.31</v>
-      </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="5">
-        <v>99.55</v>
-      </c>
-      <c r="C5" s="5">
-        <v>66.655000000000001</v>
-      </c>
-      <c r="D5" s="5">
-        <v>99.57</v>
-      </c>
-      <c r="E5" s="5">
-        <v>96.53</v>
-      </c>
-      <c r="F5" s="6">
-        <v>99.57</v>
-      </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="5">
-        <v>98.62</v>
-      </c>
-      <c r="C6" s="5">
-        <v>94.19</v>
-      </c>
-      <c r="D6" s="5">
-        <v>99.38</v>
-      </c>
-      <c r="E6" s="5">
-        <v>99.63</v>
-      </c>
-      <c r="F6" s="6">
-        <v>99.38</v>
-      </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="5">
-        <v>95.064999999999998</v>
-      </c>
-      <c r="C7" s="5">
-        <v>99.734999999999999</v>
-      </c>
-      <c r="D7" s="5">
-        <v>94.084999999999994</v>
-      </c>
-      <c r="E7" s="5">
-        <v>94.004999999999995</v>
-      </c>
-      <c r="F7" s="6">
-        <v>94.084999999999994</v>
-      </c>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="5">
-        <v>99.37</v>
-      </c>
-      <c r="C8" s="5">
-        <v>94.72</v>
-      </c>
-      <c r="D8" s="5">
-        <v>99.37</v>
-      </c>
-      <c r="E8" s="5">
-        <v>98.99</v>
-      </c>
-      <c r="F8" s="6">
-        <v>99.37</v>
-      </c>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="5">
-        <v>14.135</v>
-      </c>
-      <c r="C9" s="5">
-        <v>52.795000000000002</v>
-      </c>
-      <c r="D9" s="5">
-        <v>38.215000000000003</v>
-      </c>
-      <c r="E9" s="5">
-        <v>22.774999999999999</v>
-      </c>
-      <c r="F9" s="6">
-        <v>38.215000000000003</v>
-      </c>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="5">
-        <v>99.015000000000001</v>
-      </c>
-      <c r="C10" s="5">
-        <v>99.474999999999994</v>
-      </c>
-      <c r="D10" s="5">
-        <v>98.734999999999999</v>
-      </c>
-      <c r="E10" s="5">
-        <v>99.715000000000003</v>
-      </c>
-      <c r="F10" s="6">
-        <v>98.734999999999999</v>
-      </c>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="5">
-        <v>86.77</v>
-      </c>
-      <c r="C11" s="5">
-        <v>86.77</v>
-      </c>
-      <c r="D11" s="5">
-        <v>58.314999999999998</v>
-      </c>
-      <c r="E11" s="5">
-        <v>52.375</v>
-      </c>
-      <c r="F11" s="6">
-        <v>58.314999999999998</v>
-      </c>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="5">
-        <v>98.265000000000001</v>
-      </c>
-      <c r="C12" s="5">
-        <v>98.305000000000007</v>
-      </c>
-      <c r="D12" s="5">
-        <v>97.465000000000003</v>
-      </c>
-      <c r="E12" s="5">
-        <v>99.984999999999999</v>
-      </c>
-      <c r="F12" s="6">
-        <v>97.465000000000003</v>
-      </c>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="5">
-        <v>99.504999999999995</v>
-      </c>
-      <c r="C13" s="5">
-        <v>69.504999999999995</v>
-      </c>
-      <c r="D13" s="5">
-        <v>97.504999999999995</v>
-      </c>
-      <c r="E13" s="5">
-        <v>92.504999999999995</v>
-      </c>
-      <c r="F13" s="6">
-        <v>97.504999999999995</v>
-      </c>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="5">
-        <v>50.034999999999997</v>
-      </c>
-      <c r="C14" s="5">
-        <v>50.034999999999997</v>
-      </c>
-      <c r="D14" s="5">
-        <v>50.034999999999997</v>
-      </c>
-      <c r="E14" s="5">
-        <v>50.034999999999997</v>
-      </c>
-      <c r="F14" s="6">
-        <v>50.034999999999997</v>
-      </c>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="5">
-        <v>99.504999999999995</v>
-      </c>
-      <c r="C15" s="5">
-        <v>98.504999999999995</v>
-      </c>
-      <c r="D15" s="5">
-        <v>99.504999999999995</v>
-      </c>
-      <c r="E15" s="5">
-        <v>98.504999999999995</v>
-      </c>
-      <c r="F15" s="6">
-        <v>99.504999999999995</v>
-      </c>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="5">
-        <v>99.215000000000003</v>
-      </c>
-      <c r="C16" s="5">
-        <v>99.295000000000002</v>
-      </c>
-      <c r="D16" s="5">
-        <v>99.254999999999995</v>
-      </c>
-      <c r="E16" s="5">
-        <v>97.454999999999998</v>
-      </c>
-      <c r="F16" s="6">
-        <v>99.254999999999995</v>
-      </c>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="5">
-        <v>97.504999999999995</v>
-      </c>
-      <c r="C17" s="5">
-        <v>72.504999999999995</v>
-      </c>
-      <c r="D17" s="5">
-        <v>96.504999999999995</v>
-      </c>
-      <c r="E17" s="5">
-        <v>98.504999999999995</v>
-      </c>
-      <c r="F17" s="6">
-        <v>96.504999999999995</v>
-      </c>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="5">
-        <v>97.96</v>
-      </c>
-      <c r="C18" s="5">
-        <v>87.52</v>
-      </c>
-      <c r="D18" s="5">
-        <v>99.38</v>
-      </c>
-      <c r="E18" s="5">
-        <v>99.46</v>
-      </c>
-      <c r="F18" s="6">
-        <v>99.38</v>
-      </c>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="5">
-        <v>99.935000000000002</v>
-      </c>
-      <c r="C19" s="5">
-        <v>65.215000000000003</v>
-      </c>
-      <c r="D19" s="5">
-        <v>99.635000000000005</v>
-      </c>
-      <c r="E19" s="5">
-        <v>99.894999999999996</v>
-      </c>
-      <c r="F19" s="6">
-        <v>99.635000000000005</v>
-      </c>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="5">
-        <v>99.93</v>
-      </c>
-      <c r="C20" s="5">
-        <v>97.66</v>
-      </c>
-      <c r="D20" s="5">
+      <c r="D20" s="3">
+        <v>98.284999999999997</v>
+      </c>
+      <c r="E20" s="3">
+        <v>99.144999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="3">
+        <v>87.16</v>
+      </c>
+      <c r="C21" s="3">
+        <v>99.86</v>
+      </c>
+      <c r="D21" s="3">
+        <v>99.9</v>
+      </c>
+      <c r="E21" s="3">
+        <v>98.63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="3">
+        <v>98.89</v>
+      </c>
+      <c r="C22" s="3">
+        <v>99.23</v>
+      </c>
+      <c r="D22" s="3">
+        <v>99.16</v>
+      </c>
+      <c r="E22" s="3">
+        <v>98.53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="3">
+        <v>92.96</v>
+      </c>
+      <c r="C23" s="3">
+        <v>99.5</v>
+      </c>
+      <c r="D23" s="3">
         <v>98.86</v>
       </c>
-      <c r="E20" s="5">
-        <v>99.25</v>
-      </c>
-      <c r="F20" s="6">
-        <v>98.86</v>
-      </c>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="5">
-        <v>95.49</v>
-      </c>
-      <c r="C21" s="5">
-        <v>88.12</v>
-      </c>
-      <c r="D21" s="7">
-        <v>100</v>
-      </c>
-      <c r="E21" s="5">
-        <v>99.98</v>
-      </c>
-      <c r="F21" s="8">
-        <v>100</v>
-      </c>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="5">
-        <v>98.95</v>
-      </c>
-      <c r="C22" s="5">
-        <v>98.42</v>
-      </c>
-      <c r="D22" s="5">
-        <v>94.98</v>
-      </c>
-      <c r="E22" s="5">
-        <v>99.32</v>
-      </c>
-      <c r="F22" s="6">
-        <v>94.98</v>
-      </c>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="5">
-        <v>99.48</v>
-      </c>
-      <c r="C23" s="5">
-        <v>86.49</v>
-      </c>
-      <c r="D23" s="5">
-        <v>98.37</v>
-      </c>
-      <c r="E23" s="5">
-        <v>99.35</v>
-      </c>
-      <c r="F23" s="6">
-        <v>98.37</v>
-      </c>
-      <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="5">
-        <v>99.68</v>
+      <c r="E23" s="3">
+        <v>95.54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="4">
+        <f>AVERAGE(B2:B23)</f>
+        <v>90.920909090909078</v>
       </c>
       <c r="C24" s="5">
-        <v>76.510000000000005</v>
-      </c>
-      <c r="D24" s="5">
-        <v>99.75</v>
-      </c>
-      <c r="E24" s="5">
-        <v>99.99</v>
-      </c>
-      <c r="F24" s="6">
-        <v>99.75</v>
-      </c>
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="5">
-        <v>99.72</v>
-      </c>
-      <c r="C25" s="5">
-        <v>98.64</v>
-      </c>
-      <c r="D25" s="5">
-        <v>86.54</v>
-      </c>
-      <c r="E25" s="5">
-        <v>93.99</v>
-      </c>
-      <c r="F25" s="6">
-        <v>86.54</v>
-      </c>
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="5">
-        <v>99.4</v>
-      </c>
-      <c r="C26" s="5">
-        <v>97.405000000000001</v>
-      </c>
-      <c r="D26" s="5">
-        <v>93.745000000000005</v>
-      </c>
-      <c r="E26" s="5">
-        <v>94.704999999999998</v>
-      </c>
-      <c r="F26" s="6">
-        <v>93.745000000000005</v>
-      </c>
-      <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="5">
-        <v>98.67</v>
-      </c>
-      <c r="C27" s="5">
-        <v>86.85</v>
-      </c>
-      <c r="D27" s="5">
-        <v>98.89</v>
-      </c>
-      <c r="E27" s="5">
-        <v>99.27</v>
-      </c>
-      <c r="F27" s="6">
-        <v>98.89</v>
-      </c>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="5">
-        <v>72.155000000000001</v>
-      </c>
-      <c r="C28" s="5">
-        <v>96.314999999999998</v>
-      </c>
-      <c r="D28" s="5">
-        <v>59.895000000000003</v>
-      </c>
-      <c r="E28" s="5">
-        <v>34.325000000000003</v>
-      </c>
-      <c r="F28" s="6">
-        <v>59.895000000000003</v>
-      </c>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="5">
-        <v>60.174999999999997</v>
-      </c>
-      <c r="C29" s="5">
-        <v>39.884999999999998</v>
-      </c>
-      <c r="D29" s="5">
-        <v>99.814999999999998</v>
-      </c>
-      <c r="E29" s="5">
-        <v>99.474999999999994</v>
-      </c>
-      <c r="F29" s="6">
-        <v>99.814999999999998</v>
-      </c>
-      <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="5">
-        <v>41.445</v>
-      </c>
-      <c r="C30" s="5">
-        <v>71.924999999999997</v>
-      </c>
-      <c r="D30" s="5">
-        <v>62.805</v>
-      </c>
-      <c r="E30" s="5">
-        <v>69.245000000000005</v>
-      </c>
-      <c r="F30" s="6">
-        <v>62.805</v>
-      </c>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="5">
-        <v>85.924999999999997</v>
-      </c>
-      <c r="C31" s="5">
-        <v>99.765000000000001</v>
-      </c>
-      <c r="D31" s="5">
-        <v>66.965000000000003</v>
-      </c>
-      <c r="E31" s="5">
-        <v>64.605000000000004</v>
-      </c>
-      <c r="F31" s="6">
-        <v>66.965000000000003</v>
-      </c>
-      <c r="G31" s="4"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="5">
-        <v>99.135000000000005</v>
-      </c>
-      <c r="C32" s="5">
-        <v>93.394999999999996</v>
-      </c>
-      <c r="D32" s="5">
-        <v>99.495000000000005</v>
-      </c>
-      <c r="E32" s="5">
-        <v>91.194999999999993</v>
-      </c>
-      <c r="F32" s="6">
-        <v>99.495000000000005</v>
-      </c>
-      <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="5">
-        <v>99.92</v>
-      </c>
-      <c r="C33" s="5">
-        <v>99.3</v>
-      </c>
-      <c r="D33" s="5">
-        <v>98.54</v>
-      </c>
-      <c r="E33" s="5">
-        <v>98.58</v>
-      </c>
-      <c r="F33" s="6">
-        <v>98.54</v>
-      </c>
-      <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="5">
-        <v>99.965000000000003</v>
-      </c>
-      <c r="C34" s="5">
-        <v>91.564999999999998</v>
-      </c>
-      <c r="D34" s="5">
-        <v>99.905000000000001</v>
-      </c>
-      <c r="E34" s="5">
-        <v>99.305000000000007</v>
-      </c>
-      <c r="F34" s="6">
-        <v>99.905000000000001</v>
-      </c>
-      <c r="G34" s="4"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="5">
-        <v>99.504999999999995</v>
-      </c>
-      <c r="C35" s="5">
-        <v>90.504999999999995</v>
-      </c>
-      <c r="D35" s="5">
-        <v>98.504999999999995</v>
-      </c>
-      <c r="E35" s="5">
-        <v>94.504999999999995</v>
-      </c>
-      <c r="F35" s="6">
-        <v>98.504999999999995</v>
-      </c>
-      <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="5">
-        <v>98.935000000000002</v>
-      </c>
-      <c r="C36" s="5">
-        <v>99.965000000000003</v>
-      </c>
-      <c r="D36" s="5">
-        <v>98.555000000000007</v>
-      </c>
-      <c r="E36" s="5">
-        <v>99.224999999999994</v>
-      </c>
-      <c r="F36" s="6">
-        <v>98.555000000000007</v>
-      </c>
-      <c r="G36" s="4"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="5">
-        <v>50.005000000000003</v>
-      </c>
-      <c r="C37" s="5">
-        <v>37.005000000000003</v>
-      </c>
-      <c r="D37" s="5">
-        <v>61.005000000000003</v>
-      </c>
-      <c r="E37" s="5">
-        <v>33.005000000000003</v>
-      </c>
-      <c r="F37" s="6">
-        <v>61.005000000000003</v>
-      </c>
-      <c r="G37" s="4"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="5">
-        <v>98.84</v>
-      </c>
-      <c r="C38" s="5">
-        <v>87.16</v>
-      </c>
-      <c r="D38" s="5">
-        <v>99.3</v>
-      </c>
-      <c r="E38" s="5">
-        <v>98.98</v>
-      </c>
-      <c r="F38" s="6">
-        <v>99.3</v>
-      </c>
-      <c r="G38" s="4"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="5">
-        <v>99.12</v>
-      </c>
-      <c r="C39" s="5">
-        <v>98.89</v>
-      </c>
-      <c r="D39" s="5">
-        <v>99.97</v>
-      </c>
-      <c r="E39" s="5">
-        <v>99.78</v>
-      </c>
-      <c r="F39" s="6">
-        <v>99.97</v>
-      </c>
-      <c r="G39" s="4"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="5">
-        <v>98.09</v>
-      </c>
-      <c r="C40" s="5">
-        <v>83.06</v>
-      </c>
-      <c r="D40" s="5">
-        <v>99.77</v>
-      </c>
-      <c r="E40" s="5">
-        <v>99.38</v>
-      </c>
-      <c r="F40" s="6">
-        <v>99.77</v>
-      </c>
-      <c r="G40" s="4"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="5">
-        <v>95.06</v>
-      </c>
-      <c r="C41" s="5">
-        <v>92.96</v>
-      </c>
-      <c r="D41" s="5">
-        <v>97.44</v>
-      </c>
-      <c r="E41" s="5">
-        <v>99.87</v>
-      </c>
-      <c r="F41" s="6">
-        <v>97.44</v>
-      </c>
+        <f>AVERAGE(C2:C23)</f>
+        <v>98.763181818181792</v>
+      </c>
+      <c r="D24" s="4">
+        <f>AVERAGE(D2:D23)</f>
+        <v>97.499772727272742</v>
+      </c>
+      <c r="E24" s="4">
+        <f>AVERAGE(E2:E23)</f>
+        <v>98.182272727272732</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="20.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="9">
+        <f>_xlfn.STDEV.S(B2:B23)</f>
+        <v>9.9541799830120929</v>
+      </c>
+      <c r="C25" s="7">
+        <f t="shared" ref="C25" si="0">_xlfn.STDEV.S(C2:C23)</f>
+        <v>1.4707509787718787</v>
+      </c>
+      <c r="D25" s="10">
+        <f>_xlfn.STDEV.S(D2:D23)</f>
+        <v>2.6226529086443713</v>
+      </c>
+      <c r="E25" s="9">
+        <f>_xlfn.STDEV.S(E2:E23)</f>
+        <v>1.5189703022840098</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27"/>
+      <c r="C27"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28"/>
+      <c r="C28"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29"/>
+      <c r="C29"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30"/>
+      <c r="C30"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31"/>
+      <c r="C31"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32"/>
+      <c r="C32"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33"/>
+      <c r="C33"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34"/>
+      <c r="C34"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35"/>
+      <c r="C35"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36"/>
+      <c r="C36"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37"/>
+      <c r="C37"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38"/>
+      <c r="C38"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39"/>
+      <c r="C39"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40"/>
+      <c r="C40"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41"/>
+      <c r="C41"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42"/>
+      <c r="C42"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43"/>
+      <c r="C43"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44"/>
+      <c r="C44"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45"/>
+      <c r="C45"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46"/>
+      <c r="C46"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47"/>
+      <c r="C47"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48"/>
+      <c r="C48"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49"/>
+      <c r="C49"/>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50"/>
+      <c r="C50"/>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51"/>
+      <c r="C51"/>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52"/>
+      <c r="C52"/>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53"/>
+      <c r="C53"/>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54"/>
+      <c r="C54"/>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55"/>
+      <c r="C55"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56"/>
+      <c r="C56"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57"/>
+      <c r="C57"/>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58"/>
+      <c r="C58"/>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59"/>
+      <c r="C59"/>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60"/>
+      <c r="C60"/>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61"/>
+      <c r="C61"/>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62"/>
+      <c r="C62"/>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63"/>
+      <c r="C63"/>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64"/>
+      <c r="C64"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65"/>
+      <c r="C65"/>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66"/>
+      <c r="C66"/>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67"/>
+      <c r="C67"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:E23 B2:C23">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="between">
+      <formula>95</formula>
+      <formula>99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="greaterThan">
+      <formula>99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="22" operator="lessThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D23">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="between">
+      <formula>95</formula>
+      <formula>99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="greaterThan">
+      <formula>99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="lessThan">
+      <formula>95</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>